<commit_message>
avance mapa - fix excel
</commit_message>
<xml_diff>
--- a/data_2.xlsx
+++ b/data_2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/amondinellir_uc_cl/Documents/UC/A7/Sem 2/Visualización de Información/InfoVis-Proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{CAD53466-778C-40AD-ACFE-F23987D9904A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{993F7280-CA18-4A85-A69E-D5038A512DC0}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{CAD53466-778C-40AD-ACFE-F23987D9904A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B494A3BD-D37D-4315-8D16-40489A4DC901}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{27BD89F0-CC42-4C84-956C-74536B3DDACA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hectáreas quemadas" sheetId="1" r:id="rId1"/>
-    <sheet name="Cant incendios" sheetId="2" r:id="rId2"/>
+    <sheet name="Regiones" sheetId="3" r:id="rId1"/>
+    <sheet name="Hectáreas quemadas" sheetId="1" r:id="rId2"/>
+    <sheet name="Cant incendios" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>Año</t>
   </si>
@@ -94,6 +95,111 @@
   </si>
   <si>
     <t>Total incendios por region por año</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Arica y Parinacota</t>
+  </si>
+  <si>
+    <t>cl-2740</t>
+  </si>
+  <si>
+    <t>Tarapacá</t>
+  </si>
+  <si>
+    <t>cl-ta</t>
+  </si>
+  <si>
+    <t>Antofagasta</t>
+  </si>
+  <si>
+    <t>cl-an</t>
+  </si>
+  <si>
+    <t>Atacama</t>
+  </si>
+  <si>
+    <t>cl-at</t>
+  </si>
+  <si>
+    <t>Coquimbo</t>
+  </si>
+  <si>
+    <t>cl-co</t>
+  </si>
+  <si>
+    <t>Valparaíso</t>
+  </si>
+  <si>
+    <t>cl-vs</t>
+  </si>
+  <si>
+    <t>Región Metropolitana</t>
+  </si>
+  <si>
+    <t>cl-rm</t>
+  </si>
+  <si>
+    <t>cl-li</t>
+  </si>
+  <si>
+    <t>Maule</t>
+  </si>
+  <si>
+    <t>cl-ml</t>
+  </si>
+  <si>
+    <t>Bío-Bío</t>
+  </si>
+  <si>
+    <t>cl-bi</t>
+  </si>
+  <si>
+    <t>La Araucanía</t>
+  </si>
+  <si>
+    <t>cl-2730</t>
+  </si>
+  <si>
+    <t>Los Ríos</t>
+  </si>
+  <si>
+    <t>cl-ar</t>
+  </si>
+  <si>
+    <t>Los Lagos</t>
+  </si>
+  <si>
+    <t>cl-ll</t>
+  </si>
+  <si>
+    <t>cl-ai</t>
+  </si>
+  <si>
+    <t>cl-ma</t>
+  </si>
+  <si>
+    <t>O'Higgins</t>
+  </si>
+  <si>
+    <t>Aysén</t>
+  </si>
+  <si>
+    <t>Magallanes</t>
+  </si>
+  <si>
+    <t>Ñuble</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -360,6 +466,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,11 +788,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D4C331-8B57-4E68-BD0D-4C8F8AB09E81}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BAE634-88BC-41EC-9528-FE6CAAC9337D}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,7 +2507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D274FB4D-45EB-45A1-AF97-AC647276EDC2}">
   <dimension ref="A1:R26"/>
   <sheetViews>

</xml_diff>

<commit_message>
new tags - region
</commit_message>
<xml_diff>
--- a/data_2.xlsx
+++ b/data_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/amondinellir_uc_cl/Documents/UC/A7/Sem 2/Visualización de Información/InfoVis-Proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{CAD53466-778C-40AD-ACFE-F23987D9904A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B494A3BD-D37D-4315-8D16-40489A4DC901}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{CAD53466-778C-40AD-ACFE-F23987D9904A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D517689-0E65-4947-9168-E30E3C96CC5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{27BD89F0-CC42-4C84-956C-74536B3DDACA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{27BD89F0-CC42-4C84-956C-74536B3DDACA}"/>
   </bookViews>
   <sheets>
     <sheet name="Regiones" sheetId="3" r:id="rId1"/>
@@ -390,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -450,6 +450,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
@@ -791,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D4C331-8B57-4E68-BD0D-4C8F8AB09E81}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +963,7 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -991,10 +992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BAE634-88BC-41EC-9528-FE6CAAC9337D}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Q1"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,8 +2503,12 @@
         <v>73834.589199999988</v>
       </c>
     </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>